<commit_message>
looking at  class balance of building materials again
</commit_message>
<xml_diff>
--- a/data/Table_Deviance_Explained_2022-06-13.xlsx
+++ b/data/Table_Deviance_Explained_2022-06-13.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25718"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,25 +10,47 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B200621-BBC5-4374-902F-500B627CEAE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7125" yWindow="60" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7125" yWindow="60" windowWidth="28800" windowHeight="15435" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table_Deviance_Explained_2022-0" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Table_Deviance_Explained_2022-0'!$A$1:$G$1</definedName>
+  </definedNames>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="158">
   <si>
+    <t>Number</t>
+  </si>
+  <si>
     <t>Type</t>
   </si>
   <si>
     <t>Variable name</t>
   </si>
   <si>
+    <t>Description</t>
+  </si>
+  <si>
     <t>Deviance</t>
   </si>
   <si>
@@ -38,6 +60,18 @@
     <t>Source</t>
   </si>
   <si>
+    <t>EXP</t>
+  </si>
+  <si>
+    <t>build_near_dest</t>
+  </si>
+  <si>
+    <t>Distance to nearest destroyed building (ft)</t>
+  </si>
+  <si>
+    <t>derived from DINS</t>
+  </si>
+  <si>
     <t>CON</t>
   </si>
   <si>
@@ -47,9 +81,18 @@
     <t>Building area (ft2)</t>
   </si>
   <si>
+    <t>Land Cover</t>
+  </si>
+  <si>
     <t>build_DECKPORCHO</t>
   </si>
   <si>
+    <t>On-grade deck/porch (composite, masonry/concrete, wood, unknown, no deck/porch)</t>
+  </si>
+  <si>
+    <t>DINS</t>
+  </si>
+  <si>
     <t>build_EAVES</t>
   </si>
   <si>
@@ -95,97 +138,109 @@
     <t>parcel_year_built</t>
   </si>
   <si>
+    <t>Year built</t>
+  </si>
+  <si>
+    <t>LA County Parcel</t>
+  </si>
+  <si>
     <t>DEF</t>
   </si>
   <si>
+    <t>build_PROPANETAN</t>
+  </si>
+  <si>
+    <t>Distance to propane tank  (in feet, 0-10, 11-20, 21-30, &gt;30', unknown, no tank)</t>
+  </si>
+  <si>
+    <t>build_VEGCLEARAN</t>
+  </si>
+  <si>
+    <t>Defensible space-vegetation clearance (in feet, 0-30, 30-100, &gt;100, unknown, not applicable)</t>
+  </si>
+  <si>
+    <t>build_min_dist_shrub</t>
+  </si>
+  <si>
+    <t>Distance to nearest shrub (ft)</t>
+  </si>
+  <si>
+    <t>build_min_dist_tree</t>
+  </si>
+  <si>
+    <t>Distance to nearest tree (ft)</t>
+  </si>
+  <si>
+    <t>build_near_build</t>
+  </si>
+  <si>
+    <t>Distance to nearest building (ft)</t>
+  </si>
+  <si>
+    <t>build_overhang_ht</t>
+  </si>
+  <si>
+    <t>Average height of trees overhanging building (ft)</t>
+  </si>
+  <si>
+    <t>build_p_building_10</t>
+  </si>
+  <si>
+    <t>Percent built land cover, 10 m around building</t>
+  </si>
+  <si>
+    <t>build_p_grass_10</t>
+  </si>
+  <si>
+    <t>Percent grass land cover, 10 ft around building</t>
+  </si>
+  <si>
+    <t>build_p_otherpaved_10</t>
+  </si>
+  <si>
+    <t>Percent paved land cover, 10 ft around building</t>
+  </si>
+  <si>
+    <t>build_p_road_10</t>
+  </si>
+  <si>
+    <t>Percent road land cover, 10 ft around building</t>
+  </si>
+  <si>
+    <t>build_p_shrub_10</t>
+  </si>
+  <si>
+    <t>Percent shrub land cover, 10 ft around building</t>
+  </si>
+  <si>
+    <t>build_p_soil_10</t>
+  </si>
+  <si>
+    <t>Percent soil land cover, 10 ft around building</t>
+  </si>
+  <si>
+    <t>build_p_tree_10</t>
+  </si>
+  <si>
+    <t>Percent tree land cover, 10 ft around building</t>
+  </si>
+  <si>
+    <t>build_p_water_10</t>
+  </si>
+  <si>
+    <t>Percent water land cover, 10 ft around building</t>
+  </si>
+  <si>
+    <t>build_perc_overhang</t>
+  </si>
+  <si>
+    <t>Percent of building with trees over top</t>
+  </si>
+  <si>
     <t>build_has_tree_overhang</t>
   </si>
   <si>
-    <t>build_min_dist_shrub</t>
-  </si>
-  <si>
-    <t>Distance to nearest shrub (ft)</t>
-  </si>
-  <si>
-    <t>build_min_dist_tree</t>
-  </si>
-  <si>
-    <t>Distance to nearest tree (ft)</t>
-  </si>
-  <si>
-    <t>build_near_build</t>
-  </si>
-  <si>
-    <t>Distance to nearest building (ft)</t>
-  </si>
-  <si>
-    <t>build_overhang_ht</t>
-  </si>
-  <si>
-    <t>Average height of trees overhanging building (ft)</t>
-  </si>
-  <si>
-    <t>build_p_building_10</t>
-  </si>
-  <si>
-    <t>build_p_grass_10</t>
-  </si>
-  <si>
-    <t>Percent grass land cover, 10 ft around building</t>
-  </si>
-  <si>
-    <t>build_p_otherpaved_10</t>
-  </si>
-  <si>
-    <t>Percent paved land cover, 10 ft around building</t>
-  </si>
-  <si>
-    <t>build_p_road_10</t>
-  </si>
-  <si>
-    <t>Percent road land cover, 10 ft around building</t>
-  </si>
-  <si>
-    <t>build_p_shrub_10</t>
-  </si>
-  <si>
-    <t>Percent shrub land cover, 10 ft around building</t>
-  </si>
-  <si>
-    <t>build_p_soil_10</t>
-  </si>
-  <si>
-    <t>Percent soil land cover, 10 ft around building</t>
-  </si>
-  <si>
-    <t>build_p_tree_10</t>
-  </si>
-  <si>
-    <t>Percent tree land cover, 10 ft around building</t>
-  </si>
-  <si>
-    <t>build_p_water_10</t>
-  </si>
-  <si>
-    <t>Percent water land cover, 10 ft around building</t>
-  </si>
-  <si>
-    <t>build_perc_overhang</t>
-  </si>
-  <si>
-    <t>Percent of building with trees over top</t>
-  </si>
-  <si>
-    <t>build_PROPANETAN</t>
-  </si>
-  <si>
-    <t>Distance to propane tank  (in feet, 0-10, 11-20, 21-30, &gt;30', unknown, no tank)</t>
-  </si>
-  <si>
-    <t>build_VEGCLEARAN</t>
-  </si>
-  <si>
-    <t>Defensible space-vegetation clearance (in feet, 0-30, 30-100, &gt;100, unknown, not applicable)</t>
+    <t>Trees overhang building (binary)</t>
   </si>
   <si>
     <t>parcel_Build_P</t>
@@ -236,262 +291,163 @@
     <t>Parcel land cover- percent water</t>
   </si>
   <si>
-    <t>EXP</t>
-  </si>
-  <si>
-    <t>build_near_dest</t>
-  </si>
-  <si>
-    <t>Distance to nearest destroyed building (ft)</t>
-  </si>
-  <si>
     <t>LAND</t>
   </si>
   <si>
+    <t>build_p_building_100</t>
+  </si>
+  <si>
+    <t>Percent built land cover, 100 ft around building</t>
+  </si>
+  <si>
+    <t>build_p_building_200</t>
+  </si>
+  <si>
+    <t>Percent built land cover, 200 ft around building</t>
+  </si>
+  <si>
+    <t>build_p_building_300</t>
+  </si>
+  <si>
+    <t>Percent built land cover, 300 ft around building</t>
+  </si>
+  <si>
+    <t>build_p_grass_100</t>
+  </si>
+  <si>
+    <t>Percent grass land cover, 100 ft around building</t>
+  </si>
+  <si>
+    <t>build_p_grass_200</t>
+  </si>
+  <si>
+    <t>Percent grass land cover, 200 ft around building</t>
+  </si>
+  <si>
+    <t>build_p_grass_300</t>
+  </si>
+  <si>
+    <t>Percent grass land cover, 300 ft around building</t>
+  </si>
+  <si>
+    <t>build_p_otherpaved_100</t>
+  </si>
+  <si>
+    <t>Percent paved land cover, 100 ft around building</t>
+  </si>
+  <si>
+    <t>build_p_otherpaved_200</t>
+  </si>
+  <si>
+    <t>Percent paved land cover, 200 ft around building</t>
+  </si>
+  <si>
+    <t>build_p_otherpaved_300</t>
+  </si>
+  <si>
+    <t>Percent paved land cover, 300 ft around building</t>
+  </si>
+  <si>
+    <t>build_p_road_100</t>
+  </si>
+  <si>
+    <t>Percent road land cover, 100 ft around building</t>
+  </si>
+  <si>
+    <t>build_p_road_200</t>
+  </si>
+  <si>
+    <t>Percent road land cover, 200 ft around building</t>
+  </si>
+  <si>
+    <t>build_p_road_300</t>
+  </si>
+  <si>
+    <t>Percent road land cover, 300 ft around building</t>
+  </si>
+  <si>
+    <t>build_p_shrub_100</t>
+  </si>
+  <si>
+    <t>Percent shrub land cover, 100 ft around building</t>
+  </si>
+  <si>
+    <t>build_p_shrub_200</t>
+  </si>
+  <si>
+    <t>Percent shrub land cover, 200 ft around building</t>
+  </si>
+  <si>
+    <t>build_p_shrub_300</t>
+  </si>
+  <si>
+    <t>Percent shrub land cover, 300 ft around building</t>
+  </si>
+  <si>
+    <t>build_p_soil_100</t>
+  </si>
+  <si>
+    <t>Percent soil land cover, 100 ft around building</t>
+  </si>
+  <si>
+    <t>build_p_soil_200</t>
+  </si>
+  <si>
+    <t>Percent soil land cover, 200 ft around building</t>
+  </si>
+  <si>
+    <t>build_p_soil_300</t>
+  </si>
+  <si>
+    <t>Percent soil land cover, 300 ft around building</t>
+  </si>
+  <si>
+    <t>build_p_tree_100</t>
+  </si>
+  <si>
+    <t>Percent tree land cover, 100 ft around building</t>
+  </si>
+  <si>
+    <t>build_p_tree_200</t>
+  </si>
+  <si>
+    <t>Percent tree land cover, 200 ft around building</t>
+  </si>
+  <si>
+    <t>build_p_tree_300</t>
+  </si>
+  <si>
+    <t>Percent tree land cover, 300 ft around building</t>
+  </si>
+  <si>
+    <t>build_p_water_100</t>
+  </si>
+  <si>
+    <t>Percent water land cover, 100 ft around building</t>
+  </si>
+  <si>
+    <t>build_p_water_200</t>
+  </si>
+  <si>
+    <t>Percent water land cover, 200 ft around building</t>
+  </si>
+  <si>
+    <t>build_p_water_300</t>
+  </si>
+  <si>
+    <t>Percent water land cover, 300 ft around building</t>
+  </si>
+  <si>
+    <t>parcel_area</t>
+  </si>
+  <si>
+    <t>Parcel area (ft2)</t>
+  </si>
+  <si>
     <t>build_Mean_builddens</t>
   </si>
   <si>
-    <t>build_Mean_distall_road</t>
-  </si>
-  <si>
-    <t>Euclidian distance to any road (major and minor) (m)</t>
-  </si>
-  <si>
-    <t>build_Mean_distroad</t>
-  </si>
-  <si>
-    <t>build_p_building_100</t>
-  </si>
-  <si>
-    <t>Percent built land cover, 100 ft around building</t>
-  </si>
-  <si>
-    <t>build_p_building_200</t>
-  </si>
-  <si>
-    <t>Percent built land cover, 200 ft around building</t>
-  </si>
-  <si>
-    <t>build_p_building_300</t>
-  </si>
-  <si>
-    <t>Percent built land cover, 300 ft around building</t>
-  </si>
-  <si>
-    <t>build_p_grass_100</t>
-  </si>
-  <si>
-    <t>Percent grass land cover, 100 ft around building</t>
-  </si>
-  <si>
-    <t>build_p_grass_200</t>
-  </si>
-  <si>
-    <t>Percent grass land cover, 200 ft around building</t>
-  </si>
-  <si>
-    <t>build_p_grass_300</t>
-  </si>
-  <si>
-    <t>Percent grass land cover, 300 ft around building</t>
-  </si>
-  <si>
-    <t>build_p_otherpaved_100</t>
-  </si>
-  <si>
-    <t>Percent paved land cover, 100 ft around building</t>
-  </si>
-  <si>
-    <t>build_p_otherpaved_200</t>
-  </si>
-  <si>
-    <t>Percent paved land cover, 200 ft around building</t>
-  </si>
-  <si>
-    <t>build_p_otherpaved_300</t>
-  </si>
-  <si>
-    <t>Percent paved land cover, 300 ft around building</t>
-  </si>
-  <si>
-    <t>build_p_road_100</t>
-  </si>
-  <si>
-    <t>Percent road land cover, 100 ft around building</t>
-  </si>
-  <si>
-    <t>build_p_road_200</t>
-  </si>
-  <si>
-    <t>Percent road land cover, 200 ft around building</t>
-  </si>
-  <si>
-    <t>build_p_road_300</t>
-  </si>
-  <si>
-    <t>Percent road land cover, 300 ft around building</t>
-  </si>
-  <si>
-    <t>build_p_shrub_100</t>
-  </si>
-  <si>
-    <t>Percent shrub land cover, 100 ft around building</t>
-  </si>
-  <si>
-    <t>build_p_shrub_200</t>
-  </si>
-  <si>
-    <t>Percent shrub land cover, 200 ft around building</t>
-  </si>
-  <si>
-    <t>build_p_shrub_300</t>
-  </si>
-  <si>
-    <t>Percent shrub land cover, 300 ft around building</t>
-  </si>
-  <si>
-    <t>build_p_soil_100</t>
-  </si>
-  <si>
-    <t>Percent soil land cover, 100 ft around building</t>
-  </si>
-  <si>
-    <t>build_p_soil_200</t>
-  </si>
-  <si>
-    <t>Percent soil land cover, 200 ft around building</t>
-  </si>
-  <si>
-    <t>build_p_soil_300</t>
-  </si>
-  <si>
-    <t>Percent soil land cover, 300 ft around building</t>
-  </si>
-  <si>
-    <t>build_p_tree_100</t>
-  </si>
-  <si>
-    <t>Percent tree land cover, 100 ft around building</t>
-  </si>
-  <si>
-    <t>build_p_tree_200</t>
-  </si>
-  <si>
-    <t>Percent tree land cover, 200 ft around building</t>
-  </si>
-  <si>
-    <t>build_p_tree_300</t>
-  </si>
-  <si>
-    <t>Percent tree land cover, 300 ft around building</t>
-  </si>
-  <si>
-    <t>build_p_water_100</t>
-  </si>
-  <si>
-    <t>Percent water land cover, 100 ft around building</t>
-  </si>
-  <si>
-    <t>build_p_water_200</t>
-  </si>
-  <si>
-    <t>Percent water land cover, 200 ft around building</t>
-  </si>
-  <si>
-    <t>build_p_water_300</t>
-  </si>
-  <si>
-    <t>Percent water land cover, 300 ft around building</t>
-  </si>
-  <si>
-    <t>parcel_area</t>
-  </si>
-  <si>
-    <t>Parcel area (ft2)</t>
-  </si>
-  <si>
-    <t>TOPO</t>
-  </si>
-  <si>
-    <t>build_Mean_aspect_100m_DEM</t>
-  </si>
-  <si>
-    <t>build_Mean_aspect_30m_DEM</t>
-  </si>
-  <si>
-    <t>build_Mean_elev_100m</t>
-  </si>
-  <si>
-    <t>build_Mean_elev_30m</t>
-  </si>
-  <si>
-    <t>build_Mean_slope_100m_DEM</t>
-  </si>
-  <si>
-    <t>build_Mean_slope_30m_DEM</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>derived from DINS</t>
-  </si>
-  <si>
-    <t>Land Cover</t>
-  </si>
-  <si>
-    <t>On-grade deck/porch (composite, masonry/concrete, wood, unknown, no deck/porch)</t>
-  </si>
-  <si>
-    <t>DINS</t>
-  </si>
-  <si>
-    <t>Year built</t>
-  </si>
-  <si>
-    <t>LA County Parcel</t>
-  </si>
-  <si>
-    <t>Percent built land cover, 10 m around building</t>
-  </si>
-  <si>
-    <t>Trees overhang building (binary)</t>
-  </si>
-  <si>
-    <t>parcel_Imperv_P</t>
-  </si>
-  <si>
     <t>Interpolated housing density based on a 1-km search radius ??housing/struct</t>
-  </si>
-  <si>
-    <t>Syphard 2017</t>
-  </si>
-  <si>
-    <t>Aspect, 30 m around building</t>
-  </si>
-  <si>
-    <t>30 m DEM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aspect, 100 m around building </t>
-  </si>
-  <si>
-    <t>Elevation, 30 m around building (ft)</t>
-  </si>
-  <si>
-    <t>Elevation, 100 m around building (ft)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentage slope, 30 m around building </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentage slope, 100 m around building </t>
-  </si>
-  <si>
-    <t>Number</t>
-  </si>
-  <si>
-    <t>Euclidian distance to major road (m) </t>
   </si>
   <si>
     <r>
@@ -508,12 +464,72 @@
       <t> </t>
     </r>
   </si>
+  <si>
+    <t>build_Mean_distall_road</t>
+  </si>
+  <si>
+    <t>Euclidian distance to any road (major and minor) (m)</t>
+  </si>
+  <si>
+    <t>Syphard 2017</t>
+  </si>
+  <si>
+    <t>build_Mean_distroad</t>
+  </si>
+  <si>
+    <t>Euclidian distance to major road (m) </t>
+  </si>
+  <si>
+    <t>TOPO</t>
+  </si>
+  <si>
+    <t>build_Mean_aspect_30m_DEM</t>
+  </si>
+  <si>
+    <t>Aspect, 30 m around building</t>
+  </si>
+  <si>
+    <t>30 m DEM</t>
+  </si>
+  <si>
+    <t>build_Mean_aspect_100m_DEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aspect, 100 m around building </t>
+  </si>
+  <si>
+    <t>build_Mean_elev_30m</t>
+  </si>
+  <si>
+    <t>Elevation, 30 m around building (ft)</t>
+  </si>
+  <si>
+    <t>build_Mean_elev_100m</t>
+  </si>
+  <si>
+    <t>Elevation, 100 m around building (ft)</t>
+  </si>
+  <si>
+    <t>build_Mean_slope_30m_DEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage slope, 30 m around building </t>
+  </si>
+  <si>
+    <t>build_Mean_slope_100m_DEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage slope, 100 m around building </t>
+  </si>
+  <si>
+    <t>parcel_Imperv_P</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1374,13 +1390,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F64" sqref="F64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="23.28515625" style="1" customWidth="1"/>
@@ -1390,41 +1407,41 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>155</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>136</v>
+        <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>71</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>72</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>73</v>
+        <v>9</v>
       </c>
       <c r="E2" s="5">
         <v>23.22</v>
@@ -1433,21 +1450,21 @@
         <v>10901</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" hidden="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E3" s="5">
         <v>5.6000000000000001E-2</v>
@@ -1456,21 +1473,21 @@
         <v>10901</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" hidden="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>139</v>
+        <v>16</v>
       </c>
       <c r="E4" s="5">
         <v>0.46600000000000003</v>
@@ -1479,21 +1496,21 @@
         <v>951</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E5" s="5">
         <v>5.3570000000000002</v>
@@ -1502,21 +1519,21 @@
         <v>484</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" hidden="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E6" s="5">
         <v>0.156</v>
@@ -1525,21 +1542,21 @@
         <v>1120</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" hidden="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="E7" s="5">
         <v>1.1160000000000001</v>
@@ -1548,21 +1565,21 @@
         <v>1036</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" hidden="1">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="E8" s="5">
         <v>0.21299999999999999</v>
@@ -1571,21 +1588,21 @@
         <v>946</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" hidden="1">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="E9" s="5">
         <v>2.17</v>
@@ -1594,21 +1611,21 @@
         <v>1067</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" hidden="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="E10" s="5">
         <v>0.52800000000000002</v>
@@ -1617,21 +1634,21 @@
         <v>417</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" hidden="1">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="E11" s="5">
         <v>4.6790000000000003</v>
@@ -1640,21 +1657,21 @@
         <v>569</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" hidden="1">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>141</v>
+        <v>33</v>
       </c>
       <c r="E12" s="5">
         <v>0.01</v>
@@ -1663,21 +1680,21 @@
         <v>9900</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" hidden="1">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="E13" s="5">
         <v>1.8540000000000001</v>
@@ -1686,21 +1703,21 @@
         <v>843</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" hidden="1">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="E14" s="5">
         <v>0.96199999999999997</v>
@@ -1709,21 +1726,21 @@
         <v>1139</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" hidden="1">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="E15" s="5">
         <v>0.502</v>
@@ -1732,21 +1749,21 @@
         <v>10901</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" hidden="1">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="E16" s="5">
         <v>0.377</v>
@@ -1755,21 +1772,21 @@
         <v>10901</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" hidden="1">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="E17" s="5">
         <v>0.50700000000000001</v>
@@ -1778,21 +1795,21 @@
         <v>10901</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" hidden="1">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="E18" s="5">
         <v>0.55800000000000005</v>
@@ -1801,21 +1818,21 @@
         <v>10855</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" hidden="1">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>143</v>
+        <v>49</v>
       </c>
       <c r="E19" s="5">
         <v>0.215</v>
@@ -1824,21 +1841,21 @@
         <v>10901</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" hidden="1">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="E20" s="5">
         <v>1.325</v>
@@ -1847,21 +1864,21 @@
         <v>10901</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" hidden="1">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="E21" s="5">
         <v>0.51200000000000001</v>
@@ -1870,21 +1887,21 @@
         <v>10901</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" hidden="1">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="E22" s="5">
         <v>3.0000000000000001E-3</v>
@@ -1893,21 +1910,21 @@
         <v>10901</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" hidden="1">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="E23" s="5">
         <v>3.4000000000000002E-2</v>
@@ -1916,21 +1933,21 @@
         <v>10901</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" hidden="1">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="E24" s="5">
         <v>0.47399999999999998</v>
@@ -1939,21 +1956,21 @@
         <v>10901</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" hidden="1">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="E25" s="5">
         <v>0.83399999999999996</v>
@@ -1962,21 +1979,21 @@
         <v>10901</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" hidden="1">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="E26" s="5">
         <v>2.1999999999999999E-2</v>
@@ -1985,21 +2002,21 @@
         <v>10901</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" hidden="1">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="E27" s="5">
         <v>0.128</v>
@@ -2008,21 +2025,21 @@
         <v>10855</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" hidden="1">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>144</v>
+        <v>67</v>
       </c>
       <c r="E28" s="5">
         <v>0.26500000000000001</v>
@@ -2031,21 +2048,21 @@
         <v>10855</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="E29" s="5">
         <v>6.9649999999999999</v>
@@ -2054,21 +2071,21 @@
         <v>10901</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" hidden="1">
       <c r="A30" s="1">
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="E30" s="5">
         <v>2.706</v>
@@ -2077,21 +2094,21 @@
         <v>10901</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" hidden="1">
       <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="E31" s="5">
         <v>3.218</v>
@@ -2100,21 +2117,21 @@
         <v>10901</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" hidden="1">
       <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="E32" s="5">
         <v>3.746</v>
@@ -2123,21 +2140,21 @@
         <v>10901</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" hidden="1">
       <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="E33" s="5">
         <v>0.129</v>
@@ -2146,21 +2163,21 @@
         <v>10901</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" hidden="1">
       <c r="A34" s="1">
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="E34" s="5">
         <v>1.7509999999999999</v>
@@ -2169,21 +2186,21 @@
         <v>10901</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" hidden="1">
       <c r="A35" s="1">
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="E35" s="5">
         <v>1.29</v>
@@ -2192,21 +2209,21 @@
         <v>10901</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" hidden="1">
       <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="E36" s="5">
         <v>8.7999999999999995E-2</v>
@@ -2215,21 +2232,21 @@
         <v>10901</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" hidden="1">
       <c r="A37" s="1">
         <v>37</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="E37" s="5">
         <v>3.81</v>
@@ -2238,21 +2255,21 @@
         <v>10901</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" hidden="1">
       <c r="A38" s="1">
         <v>38</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="E38" s="5">
         <v>4.9939999999999998</v>
@@ -2261,21 +2278,21 @@
         <v>10901</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" s="1">
         <v>39</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="E39" s="5">
         <v>5.3810000000000002</v>
@@ -2284,21 +2301,21 @@
         <v>10901</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" hidden="1">
       <c r="A40" s="1">
         <v>40</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="E40" s="5">
         <v>2.097</v>
@@ -2307,21 +2324,21 @@
         <v>10901</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" hidden="1">
       <c r="A41" s="1">
         <v>41</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="E41" s="5">
         <v>2.92</v>
@@ -2330,21 +2347,21 @@
         <v>10901</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" hidden="1">
       <c r="A42" s="1">
         <v>42</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="E42" s="5">
         <v>3.6150000000000002</v>
@@ -2353,21 +2370,21 @@
         <v>10901</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" hidden="1">
       <c r="A43" s="1">
         <v>43</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="E43" s="5">
         <v>3.117</v>
@@ -2376,21 +2393,21 @@
         <v>10901</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" hidden="1">
       <c r="A44" s="1">
         <v>44</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E44" s="5">
         <v>4.9640000000000004</v>
@@ -2399,21 +2416,21 @@
         <v>10901</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" s="1">
         <v>45</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="E45" s="5">
         <v>5.9429999999999996</v>
@@ -2422,21 +2439,21 @@
         <v>10901</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" hidden="1">
       <c r="A46" s="1">
         <v>46</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="E46" s="5">
         <v>2.266</v>
@@ -2445,21 +2462,21 @@
         <v>10901</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" hidden="1">
       <c r="A47" s="1">
         <v>47</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="E47" s="5">
         <v>3.238</v>
@@ -2468,21 +2485,21 @@
         <v>10901</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" hidden="1">
       <c r="A48" s="1">
         <v>48</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="E48" s="5">
         <v>4.1779999999999999</v>
@@ -2491,21 +2508,21 @@
         <v>10901</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" hidden="1">
       <c r="A49" s="1">
         <v>49</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="E49" s="5">
         <v>0.14099999999999999</v>
@@ -2514,21 +2531,21 @@
         <v>10901</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" hidden="1">
       <c r="A50" s="1">
         <v>50</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="E50" s="5">
         <v>0.59299999999999997</v>
@@ -2537,21 +2554,21 @@
         <v>10901</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" hidden="1">
       <c r="A51" s="1">
         <v>51</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="E51" s="5">
         <v>1.1950000000000001</v>
@@ -2560,21 +2577,21 @@
         <v>10901</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" hidden="1">
       <c r="A52" s="1">
         <v>52</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="E52" s="5">
         <v>2.2109999999999999</v>
@@ -2583,21 +2600,21 @@
         <v>10901</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" hidden="1">
       <c r="A53" s="1">
         <v>53</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="E53" s="5">
         <v>2.7930000000000001</v>
@@ -2606,21 +2623,21 @@
         <v>10901</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" hidden="1">
       <c r="A54" s="1">
         <v>54</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="E54" s="5">
         <v>2.4009999999999998</v>
@@ -2629,21 +2646,21 @@
         <v>10901</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" hidden="1">
       <c r="A55" s="1">
         <v>55</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="E55" s="5">
         <v>2.5979999999999999</v>
@@ -2652,21 +2669,21 @@
         <v>10901</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" hidden="1">
       <c r="A56" s="1">
         <v>56</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="E56" s="5">
         <v>2.266</v>
@@ -2675,21 +2692,21 @@
         <v>10901</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" hidden="1">
       <c r="A57" s="1">
         <v>57</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="E57" s="5">
         <v>2.4729999999999999</v>
@@ -2698,21 +2715,21 @@
         <v>10901</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" hidden="1">
       <c r="A58" s="1">
         <v>58</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="E58" s="5">
         <v>6.9000000000000006E-2</v>
@@ -2721,21 +2738,21 @@
         <v>10901</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" hidden="1">
       <c r="A59" s="1">
         <v>59</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="E59" s="5">
         <v>3.3000000000000002E-2</v>
@@ -2744,21 +2761,21 @@
         <v>10901</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" hidden="1">
       <c r="A60" s="1">
         <v>60</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="E60" s="5">
         <v>4.2999999999999997E-2</v>
@@ -2767,21 +2784,21 @@
         <v>10901</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" hidden="1">
       <c r="A61" s="1">
         <v>61</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="E61" s="5">
         <v>0.314</v>
@@ -2790,21 +2807,21 @@
         <v>10901</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" hidden="1">
       <c r="A62" s="1">
         <v>62</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>75</v>
+        <v>135</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="E62" s="5">
         <v>2.2410000000000001</v>
@@ -2813,21 +2830,21 @@
         <v>10828</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" hidden="1">
       <c r="A63" s="1">
         <v>63</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>76</v>
+        <v>138</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>77</v>
+        <v>139</v>
       </c>
       <c r="E63" s="5">
         <v>0.14899999999999999</v>
@@ -2836,21 +2853,21 @@
         <v>10901</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" hidden="1">
       <c r="A64" s="1">
         <v>64</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>78</v>
+        <v>141</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="E64" s="5">
         <v>1.2789999999999999</v>
@@ -2859,21 +2876,21 @@
         <v>10828</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" hidden="1">
       <c r="A65" s="1">
         <v>65</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E65" s="5">
         <v>0.10199999999999999</v>
@@ -2882,21 +2899,21 @@
         <v>10901</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" hidden="1">
       <c r="A66" s="1">
         <v>66</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E66" s="5">
         <v>0.17599999999999999</v>
@@ -2905,21 +2922,21 @@
         <v>10901</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" hidden="1">
       <c r="A67" s="1">
         <v>67</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E67" s="5">
         <v>5.8000000000000003E-2</v>
@@ -2928,18 +2945,18 @@
         <v>10901</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" hidden="1">
       <c r="A68" s="1">
         <v>68</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>132</v>
+        <v>151</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>152</v>
@@ -2951,21 +2968,21 @@
         <v>10901</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" hidden="1">
       <c r="A69" s="1">
         <v>69</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>135</v>
+        <v>153</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E69" s="5">
         <v>3.5939999999999999</v>
@@ -2974,21 +2991,21 @@
         <v>10901</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" hidden="1">
       <c r="A70" s="1">
         <v>70</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E70" s="5">
         <v>4.5380000000000003</v>
@@ -2997,10 +3014,17 @@
         <v>10901</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G70" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="4">
+      <customFilters>
+        <customFilter operator="greaterThanOrEqual" val="5"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S74">
     <sortCondition ref="A2:A74"/>
   </sortState>
@@ -3013,250 +3037,250 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>